<commit_message>
server list page executed
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/ad_blocking_ server/ad_blocking_ server.xlsx
+++ b/apps/features/backlog/android/ad_blocking_ server/ad_blocking_ server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\ad_blocking_ server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD668463-ACD4-41B0-9F2D-D2ADBEF287C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF3B3F-7346-4661-9AA7-1D975FBD735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Prerequisites</t>
   </si>
@@ -66,10 +66,6 @@
     <t>check ad blocking consistency</t>
   </si>
   <si>
-    <t>ad blocking should be consistently applied across 
-different servers</t>
-  </si>
-  <si>
     <t>check the impact on page load time</t>
   </si>
   <si>
@@ -92,9 +88,6 @@
   </si>
   <si>
     <t>check ad blocking on different browsers</t>
-  </si>
-  <si>
-    <t>check ad blocking on mobile devices</t>
   </si>
   <si>
     <t>should confirm that the ad-blocking feature is 
@@ -133,102 +126,6 @@
 is consistent across various browsers</t>
   </si>
   <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check the visibility of ad blocking servers</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check the dynamic ad blocking</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to connect to multiple servers from the "ad blocking server" list</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to measure the impact of ad blocking on the overall page load time</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check if the user interface provides information about the ad-blocking status when connected to an "ad blocking server."</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check if the application allows users to customize ad-blocking settings (e.g., whitelist certain domains)</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test the ad-blocking servers with different web browsers (e.g., Chrome, Firefox)</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check ad blocking on mobile devices</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to Connect to an "ad blocking server" and visit websites known for displaying ads</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test ad-blocking with various ad formats, including banners, pop-ups, and video ads</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test the ad-blocking servers with websites using https</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to simulate a high number of users connecting to ad-blocking servers simultaneously</t>
-  </si>
-  <si>
     <t>test Case ID</t>
   </si>
   <si>
@@ -245,96 +142,6 @@
   </si>
   <si>
     <t>try to see ads on server no.1 for ad-blocking servers with the https://bangla.bdnews24.com/ news website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page.
-6. select the first ad-blocking server from the ad-blocking section.
-7. visit  bangla.bdnew24.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. select the first ad-blocking server from the ad-blocking section.
-7. visit  prothomalo.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page.
-6. select the first ad-blocking server from the ad-blocking section.
-7. visit  cricinfo.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page.
-6. select the second ad-blocking server from the ad-blocking section.
-7. visit  bangla.bdnew24.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. select the second ad-blocking server from the ad-blocking section.
-7. visit  prothomalo.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page.
-6. select the second ad-blocking server from the ad-blocking section.
-7. visit  cricinfo.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page.
-6. select the third ad-blocking server from the ad-blocking section.
-7. visit  bangla.bdnew24.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. Enter your password in the password field.
-4. tap the login button
-5. navigate to the server list page.
-6. select the third ad-blocking server from the ad-blocking section.
-7. visit  bangla.bdnew24.com
-8. start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. go to the google app store and install symlexvpn on your device
-2. open the symlexvpn application once it's installed.
-3. Enter your password in the password field.
-4. tap the login button
-5. navigate to the server list page.
-6. select the third ad-blocking server from the ad-blocking section.
-7. visit  cricinfo.com
-8. start browsing the website.</t>
   </si>
   <si>
     <t>try to see ads the server no.1 for ads blocking server with the  prothomalo.com news website</t>
@@ -426,6 +233,217 @@
   <si>
     <t>TC_SYM_ABS_021</t>
   </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page.
+6. select the first ad-blocking server from the ad-blocking section.
+7. visit  bangla.bdnew24.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. select the first ad-blocking server from the ad-blocking section.
+7. visit  prothomalo.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page.
+6. select the first ad-blocking server from the ad-blocking section.
+7. visit  cricinfo.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page.
+6. select the second ad-blocking server from the ad-blocking section.
+7. visit  bangla.bdnew24.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. select the second ad-blocking server from the ad-blocking section.
+7. visit  prothomalo.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page.
+6. select the second ad-blocking server from the ad-blocking section.
+7. visit  cricinfo.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page.
+6. select the third ad-blocking server from the ad-blocking section.
+7. visit  bangla.bdnew24.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. Enter your password in the password field.
+4. tap the login button
+5. navigate to the server list page.
+6. select the third ad-blocking server from the ad-blocking section.
+7. visit  bangla.bdnew24.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. Enter your password in the password field.
+4. tap the login button
+5. navigate to the server list page.
+6. select the third ad-blocking server from the ad-blocking section.
+7. visit  cricinfo.com
+8. start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check the visibility of ad blocking servers</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to connect to multiple servers from the "ad blocking server" list</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to measure the impact of ad blocking on the overall page load time</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check if the user interface provides information about the ad-blocking status when connected to an "ad blocking server."</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check if the application allows users to customize ad-blocking settings (e.g., whitelist certain domains)</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test the ad-blocking servers with different web browsers (e.g., Chrome, Firefox)</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test ad-blocking with various ad formats, including banners, pop-ups, and video ads</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test the ad-blocking servers with websites using https</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to simulate a high number of users connecting to ad-blocking servers simultaneously</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. connect to any ad blocking server 
+6. try to check the dynamic ad blocking</t>
+  </si>
+  <si>
+    <t>one server should be coonected each time</t>
+  </si>
+  <si>
+    <t>check ad blocking on different devices</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check ad blocking on different devices</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to Connect to an "ad blocking server" and visit websites known for displaying ads
+7. check user feedback for ad blocking</t>
+  </si>
+  <si>
+    <t>TC_SYM_ABS_022</t>
+  </si>
+  <si>
+    <t>check the DNS leak</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page. and connect to any server
+6. goto browser , check DNS leak on ip-score website</t>
+  </si>
+  <si>
+    <t>should not be leaked</t>
+  </si>
 </sst>
 </file>
 
@@ -479,7 +497,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +514,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -601,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -653,6 +677,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1380,7 +1416,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G24" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G25" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1598,8 +1634,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1653,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1675,16 +1711,16 @@
     </row>
     <row r="3" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1</v>
@@ -1717,19 +1753,19 @@
     </row>
     <row r="4" spans="1:26" ht="161.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>5</v>
@@ -1759,19 +1795,19 @@
     </row>
     <row r="5" spans="1:26" ht="159.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>5</v>
@@ -1801,19 +1837,19 @@
     </row>
     <row r="6" spans="1:26" ht="162.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>5</v>
@@ -1841,19 +1877,19 @@
     </row>
     <row r="7" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>5</v>
@@ -1881,19 +1917,19 @@
     </row>
     <row r="8" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>5</v>
@@ -1921,19 +1957,19 @@
     </row>
     <row r="9" spans="1:26" ht="160.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>5</v>
@@ -1961,19 +1997,19 @@
     </row>
     <row r="10" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>5</v>
@@ -2001,19 +2037,19 @@
     </row>
     <row r="11" spans="1:26" ht="156.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>5</v>
@@ -2041,19 +2077,19 @@
     </row>
     <row r="12" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>5</v>
@@ -2081,7 +2117,7 @@
     </row>
     <row r="13" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>6</v>
@@ -2090,7 +2126,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
@@ -2121,7 +2157,7 @@
     </row>
     <row r="14" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -2130,7 +2166,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>10</v>
@@ -2161,7 +2197,7 @@
     </row>
     <row r="15" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>6</v>
@@ -2170,10 +2206,10 @@
         <v>11</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>5</v>
@@ -2201,19 +2237,19 @@
     </row>
     <row r="16" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>5</v>
@@ -2241,19 +2277,19 @@
     </row>
     <row r="17" spans="1:26" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>5</v>
@@ -2281,22 +2317,22 @@
     </row>
     <row r="18" spans="1:26" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F18" s="9" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="1"/>
@@ -2321,19 +2357,19 @@
     </row>
     <row r="19" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>5</v>
@@ -2361,19 +2397,19 @@
     </row>
     <row r="20" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>5</v>
@@ -2399,21 +2435,21 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>5</v>
@@ -2441,19 +2477,19 @@
     </row>
     <row r="22" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>5</v>
@@ -2481,19 +2517,19 @@
     </row>
     <row r="23" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>5</v>
@@ -2521,22 +2557,22 @@
     </row>
     <row r="24" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>66</v>
+      <c r="F24" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="1"/>
@@ -2559,14 +2595,26 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+    <row r="25" spans="1:26" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="20"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -29612,7 +29660,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:F17 F19:F23" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:F17 F19:F25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F5" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
shadowsock connection and promet vpn check
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/ad_blocking_ server/ad_blocking_ server.xlsx
+++ b/apps/features/backlog/android/ad_blocking_ server/ad_blocking_ server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\ad_blocking_ server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF3B3F-7346-4661-9AA7-1D975FBD735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB83AA8-7A88-4F26-A2F1-9394C6CEA4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
   <si>
     <t>Prerequisites</t>
   </si>
@@ -444,6 +444,70 @@
   <si>
     <t>should not be leaked</t>
   </si>
+  <si>
+    <t>TC_SYM_ABS_023</t>
+  </si>
+  <si>
+    <t>check if the server is adding to favourite server list or not</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page, add any ad block server to favourite 
+6. check if the server is adding to favourite server list or not</t>
+  </si>
+  <si>
+    <t>should be added</t>
+  </si>
+  <si>
+    <t>TC_SYM_ABS_024</t>
+  </si>
+  <si>
+    <t>check if removing from favourite server list , also remove the fav icon from ad blocking server list and vice versa</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list
+6. check if removing from favourite server list , also remove the fav icon from ad blocking server list and vice versa</t>
+  </si>
+  <si>
+    <t>should work properly</t>
+  </si>
+  <si>
+    <t>TC_SYM_ABS_025</t>
+  </si>
+  <si>
+    <t>check if the dropdown of the ad blocking server is working properly or not</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page
+6. check if the dropdown of the ad blocking server is working 
+properly or not</t>
+  </si>
+  <si>
+    <t>TC_SYM_ABS_026</t>
+  </si>
+  <si>
+    <t>check click on emoji/text/arrow sign, dropdown is happening or not</t>
+  </si>
+  <si>
+    <t>1. go to the google play store and install symlexvpn on your device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page , check ad blocking server,
+6. click on emoji/text/arrow sign
+7. dropdown should be happened</t>
+  </si>
 </sst>
 </file>
 
@@ -660,6 +724,18 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,18 +753,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,7 +1480,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G25" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G29" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1634,8 +1698,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1652,15 +1716,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1682,13 +1746,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2322,7 +2386,7 @@
       <c r="B18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -2596,25 +2660,25 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="13" t="s">
         <v>91</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="20"/>
+      <c r="G25" s="14"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2635,14 +2699,26 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+    <row r="26" spans="1:26" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="14"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2663,14 +2739,26 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+    <row r="27" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="14"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2691,14 +2779,26 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+    <row r="28" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="14"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2719,14 +2819,26 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+    <row r="29" spans="1:26" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="14"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>

</xml_diff>